<commit_message>
negfin c++ corr 1
</commit_message>
<xml_diff>
--- a/Python/datasets/Experiments/ARMDatasetFeatures.xlsx
+++ b/Python/datasets/Experiments/ARMDatasetFeatures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\WebApriori\Python\datasets\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30344D61-96AF-444E-9BD4-661A5632A6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D661032A-0448-44FD-8D79-73ED3CFF2C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -630,7 +630,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>